<commit_message>
Added maintenance and deployment plan, updated hours
</commit_message>
<xml_diff>
--- a/documentation/project4_hours.xlsx
+++ b/documentation/project4_hours.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/landen/Desktop/Classes/Spring22/eecs448/Project4/ds_visualizerProject4/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eef0d66f1688d40a/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4830679-0F2C-E147-B16A-D318C2B53246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{E4830679-0F2C-E147-B16A-D318C2B53246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0B039E1-5B89-495D-B21B-F17C3FFF449E}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="1600" windowWidth="27720" windowHeight="15840" xr2:uid="{095FDC74-654F-AD46-9E96-47D17C496F71}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11295" xr2:uid="{095FDC74-654F-AD46-9E96-47D17C496F71}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>Landen</t>
+  </si>
+  <si>
+    <t>Duy</t>
   </si>
 </sst>
 </file>
@@ -423,19 +426,19 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -446,7 +449,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -457,7 +460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -468,7 +471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -479,7 +482,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -490,55 +493,63 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44672</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C15">
         <f>SUM(C3:C14)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
     </row>
   </sheetData>

</xml_diff>